<commit_message>
Form M amended to add party_id
</commit_message>
<xml_diff>
--- a/M_objeccoes_correcoes/LEGEND_M_objeccoes_correcoes-media/LEGEND_M_objeccoes_correcoes.xlsx
+++ b/M_objeccoes_correcoes/LEGEND_M_objeccoes_correcoes-media/LEGEND_M_objeccoes_correcoes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11610" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11610" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2627" uniqueCount="1214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="1209">
   <si>
     <t>type</t>
   </si>
@@ -3182,9 +3182,6 @@
     <t>${tec_nome}='Outro'</t>
   </si>
   <si>
-    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâê]{1,25}$")</t>
-  </si>
-  <si>
     <t>assoc_id</t>
   </si>
   <si>
@@ -3338,9 +3335,6 @@
     <t>LEGEND M Objeccoes e Correcoes</t>
   </si>
   <si>
-    <t>LEGEND_M_V1</t>
-  </si>
-  <si>
     <t>"Registo de Objecções e Correções"</t>
   </si>
   <si>
@@ -3572,109 +3566,101 @@
     <t>Mahi Orera [Manla]</t>
   </si>
   <si>
-    <t>nasc</t>
-  </si>
-  <si>
-    <t>val</t>
-  </si>
-  <si>
-    <t>selected(${issues}, 'nasc')</t>
-  </si>
-  <si>
-    <t>selected(${issues}, 'val')</t>
-  </si>
-  <si>
-    <t>pessoa_dob_new</t>
-  </si>
-  <si>
-    <t>pessoa_idval_new</t>
-  </si>
-  <si>
-    <t>Novo data de nascimento</t>
-  </si>
-  <si>
-    <t>Novo apelido da pessoa:</t>
-  </si>
-  <si>
-    <t>Novo nome da pessoa:</t>
-  </si>
-  <si>
-    <t>Mudar o tipo de documento de identificação:</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>no-calendar</t>
-  </si>
-  <si>
-    <t>Novo data de validade de documento</t>
-  </si>
-  <si>
     <t>outcomes</t>
   </si>
   <si>
-    <t>Confirmado pelo requerente, sem mudanças</t>
-  </si>
-  <si>
-    <t>Confirmado pelo requerente, com mudanças</t>
-  </si>
-  <si>
-    <t>Disputado, não pode ser certificado agora</t>
-  </si>
-  <si>
-    <t>Não confirmado pelo requerente, mas sem objecções</t>
-  </si>
-  <si>
-    <t>conf</t>
-  </si>
-  <si>
-    <t>disp</t>
-  </si>
-  <si>
-    <t>conf_mudar</t>
-  </si>
-  <si>
-    <t>no_conf</t>
-  </si>
-  <si>
     <t>select_one outcomes</t>
   </si>
   <si>
-    <t>resultado</t>
-  </si>
-  <si>
-    <t>Selecionar o resultado do processo de Confirmações, Objecções e Correções</t>
-  </si>
-  <si>
-    <t>${resultado}='conf_mudar'</t>
-  </si>
-  <si>
-    <t>Mudar a data de nascimento:</t>
-  </si>
-  <si>
-    <t>Mudar o numero de documento:</t>
-  </si>
-  <si>
-    <t>Mudar a validade de documento de identificação:</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
-    <t>limites_foto</t>
-  </si>
-  <si>
-    <t>Tire uma fotografia do mapa, mostrando a mudanca dos limites da parcela</t>
-  </si>
-  <si>
-    <t>concat('COC','_',${found_pov},'_',${parcel_id})</t>
+    <t>LEGEND_M_V2</t>
+  </si>
+  <si>
+    <t>concat('OC','_',${parcel_id})</t>
   </si>
   <si>
     <t>&lt;br/&gt; &lt;span style="color:#57b055"&gt;${my_form_name}&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;Este formulário é utilizado para gravar os resultados de processo de Objecções e Correções.
 O técnico pode usar o formulário &lt;br/&gt; &lt;span style="color:#57b055"&gt;depois de conclusão da publicação do edital&lt;/span&gt;.
-O formulário é usado para reportar a necessidade de mudar algo, seja a configuração das parcelas ou seja mudanças na informação relacionada com os titulares.  Também é necessário para fazer registo de confirmação do titular - assim, o formulário é preenchido uma vez para cada parcela que foi publicada.
+O formulário é usado para reportar a necessidade de mudar ou a configuração das parcelas ou mudanças na informação relacionada sobre os titulares. 
+&lt;span style="color:#FF0000"&gt;Se os detalhes de mais de um titular dos co-titulares precisam de ser alterados, o formulário deve ser preenchido uma vez para cada titular&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;
 Por favor deslizar para a frente para continuar.</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>Por favor, selecione o resultado para esta parcela</t>
+  </si>
+  <si>
+    <t>party_id</t>
+  </si>
+  <si>
+    <t>Qual é o numero do (co-)titular?</t>
+  </si>
+  <si>
+    <t>party_id_check</t>
+  </si>
+  <si>
+    <t>Por favor, re-digite o número do (co-)titular como confirmação:</t>
+  </si>
+  <si>
+    <t>.=${party_id}</t>
+  </si>
+  <si>
+    <t>O número do titular que reentrou não corresponde à sua primeira entrada. Faça a favor de verificar de novo.</t>
+  </si>
+  <si>
+    <t>${outcome}='change'</t>
+  </si>
+  <si>
+    <t>Novo apelido da pessoa</t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâôàèê]{1,75}$")</t>
+  </si>
+  <si>
+    <t>Resposta invalida - O campo do nome não pode incluir um novo paragrafo. Faça a favor de eliminar qualquer linha adicional.</t>
+  </si>
+  <si>
+    <t>Novo nome da pessoa</t>
+  </si>
+  <si>
+    <t>Mudar o tipo de documento de identificação</t>
+  </si>
+  <si>
+    <t>limites_new_image</t>
+  </si>
+  <si>
+    <t>Tire uma fotografia da parcela no mapa, mostrando claramente a mudança nas limites</t>
+  </si>
+  <si>
+    <t>Mudar o numero de documento</t>
+  </si>
+  <si>
+    <t>certify</t>
+  </si>
+  <si>
+    <t>Todos os detalhes estão corretos e confirmados</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>Foi feita uma alteração aos detalhes do(s) (co-)titular(es) ou as limites da parcela</t>
+  </si>
+  <si>
+    <t>disputed</t>
+  </si>
+  <si>
+    <t>Foi feita uma objecção que necessita uma resolução ainda</t>
+  </si>
+  <si>
+    <t>unconfirmed</t>
+  </si>
+  <si>
+    <t>O titular não confirmou os seus detalhes durante o período de O &amp; C</t>
   </si>
 </sst>
 </file>
@@ -4097,7 +4083,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4280,8 +4266,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -4289,10 +4275,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="239">
@@ -4873,11 +4862,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4887,9 +4876,9 @@
     <col min="3" max="3" width="65.125" style="8" customWidth="1"/>
     <col min="4" max="4" width="17.625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="8" customWidth="1"/>
     <col min="7" max="7" width="27.75" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.875" style="8" customWidth="1"/>
     <col min="9" max="9" width="41.875" style="8" customWidth="1"/>
     <col min="10" max="10" width="7.625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.5" style="8" bestFit="1" customWidth="1"/>
@@ -4963,7 +4952,7 @@
         <v>1044</v>
       </c>
       <c r="M4" s="58" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="40" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4973,8 +4962,8 @@
       <c r="B5" s="48" t="s">
         <v>1046</v>
       </c>
-      <c r="C5" s="95" t="s">
-        <v>1213</v>
+      <c r="C5" s="90" t="s">
+        <v>1183</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -5007,8 +4996,11 @@
       <c r="G7" s="40" t="s">
         <v>1049</v>
       </c>
-      <c r="H7" s="45" t="s">
-        <v>1050</v>
+      <c r="H7" s="89" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I7" s="89" t="s">
+        <v>1195</v>
       </c>
       <c r="J7" s="40" t="s">
         <v>21</v>
@@ -5073,13 +5065,13 @@
     </row>
     <row r="11" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C11" s="45" t="s">
         <v>1053</v>
-      </c>
-      <c r="B11" s="49" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>1054</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>1030</v>
@@ -5093,19 +5085,19 @@
     </row>
     <row r="12" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C12" s="60" t="s">
         <v>1104</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>1105</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>1106</v>
       </c>
       <c r="J12" s="57" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="61" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
@@ -5113,10 +5105,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="59" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C13" s="57" t="s">
         <v>1111</v>
-      </c>
-      <c r="C13" s="57" t="s">
-        <v>1113</v>
       </c>
       <c r="E13" s="57"/>
       <c r="F13" s="57"/>
@@ -5125,7 +5117,7 @@
         <v>21</v>
       </c>
       <c r="L13" s="58" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.25">
@@ -5133,208 +5125,246 @@
         <v>28</v>
       </c>
       <c r="B14" s="59" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>1113</v>
+      </c>
+      <c r="H14" s="57" t="s">
         <v>1114</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="I14" s="57" t="s">
         <v>1115</v>
-      </c>
-      <c r="H14" s="57" t="s">
-        <v>1116</v>
-      </c>
-      <c r="I14" s="57" t="s">
-        <v>1117</v>
       </c>
       <c r="J14" s="57" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="57" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89" t="s">
-        <v>1202</v>
+        <v>1179</v>
       </c>
       <c r="B15" s="91" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C15" s="89" t="s">
-        <v>1204</v>
+        <v>1184</v>
+      </c>
+      <c r="C15" s="92" t="s">
+        <v>1185</v>
       </c>
       <c r="J15" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="89" t="s">
+    </row>
+    <row r="16" spans="1:15" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="91" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C16" s="89" t="s">
+        <v>1187</v>
+      </c>
+      <c r="J16" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="93" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="91" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C17" s="92" t="s">
+        <v>1189</v>
+      </c>
+      <c r="H17" s="89" t="s">
+        <v>1190</v>
+      </c>
+      <c r="I17" s="89" t="s">
+        <v>1191</v>
+      </c>
+      <c r="J17" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="93" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B18" s="91" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C18" s="92" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G18" s="93" t="s">
+        <v>1192</v>
+      </c>
+      <c r="J18" s="89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="91" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C19" s="92" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G19" s="89" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H19" s="89" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I19" s="89" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J19" s="89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C20" s="92" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G20" s="89" t="s">
+        <v>1170</v>
+      </c>
+      <c r="H20" s="89" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I20" s="89" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J20" s="89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="89" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C21" s="92" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G21" s="89" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J21" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="93" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
-        <v>1118</v>
-      </c>
-      <c r="B16" s="59" t="s">
-        <v>1119</v>
-      </c>
-      <c r="C16" s="60" t="s">
-        <v>1124</v>
-      </c>
-      <c r="G16" s="94" t="s">
-        <v>1205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
+    <row r="22" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B22" s="91" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C22" s="92" t="s">
+        <v>1197</v>
+      </c>
+      <c r="G22" s="89" t="s">
+        <v>1172</v>
+      </c>
+      <c r="J22" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="93" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="59" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C17" s="92" t="s">
-        <v>1187</v>
-      </c>
-      <c r="G17" s="57" t="s">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="59" t="s">
-        <v>1160</v>
-      </c>
-      <c r="C18" s="92" t="s">
-        <v>1188</v>
-      </c>
-      <c r="G18" s="57" t="s">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
-        <v>1131</v>
-      </c>
-      <c r="B19" s="59" t="s">
+      <c r="B23" s="91" t="s">
         <v>1161</v>
       </c>
-      <c r="C19" s="60" t="s">
-        <v>1125</v>
-      </c>
-      <c r="G19" s="57" t="s">
+      <c r="C23" s="89" t="s">
+        <v>1154</v>
+      </c>
+      <c r="G23" s="89" t="s">
         <v>1173</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="H23" s="89" t="s">
         <v>1155</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="I23" s="89" t="s">
+        <v>1156</v>
+      </c>
+      <c r="J23" s="89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="89" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B24" s="91" t="s">
         <v>1162</v>
       </c>
-      <c r="C20" s="92" t="s">
-        <v>1189</v>
-      </c>
-      <c r="G20" s="57" t="s">
+      <c r="C24" s="92" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G24" s="89" t="s">
         <v>1174</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="59" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>1156</v>
-      </c>
-      <c r="G21" s="57" t="s">
+      <c r="J24" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="89" t="s">
         <v>1175</v>
       </c>
-      <c r="H21" s="57" t="s">
-        <v>1157</v>
-      </c>
-      <c r="I21" s="57" t="s">
-        <v>1158</v>
-      </c>
-      <c r="J21" s="57" t="s">
+    </row>
+    <row r="25" spans="1:13" s="89" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="89" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C25" s="92" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G25" s="89" t="s">
+        <v>1174</v>
+      </c>
+      <c r="J25" s="89" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="s">
-        <v>1190</v>
-      </c>
-      <c r="B22" s="91" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C22" s="89" t="s">
-        <v>1186</v>
-      </c>
-      <c r="G22" s="89" t="s">
-        <v>1182</v>
-      </c>
-      <c r="L22" s="57" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
-        <v>1190</v>
-      </c>
-      <c r="B23" s="91" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C23" s="89" t="s">
-        <v>1192</v>
-      </c>
-      <c r="G23" s="89" t="s">
-        <v>1183</v>
-      </c>
-      <c r="L23" s="57" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
-        <v>1209</v>
-      </c>
-      <c r="B24" s="91" t="s">
-        <v>1210</v>
-      </c>
-      <c r="C24" s="94" t="s">
-        <v>1211</v>
-      </c>
-      <c r="G24" s="89" t="s">
-        <v>1176</v>
-      </c>
-      <c r="I24" s="89"/>
-      <c r="J24" s="94" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B25" s="59" t="s">
-        <v>1164</v>
-      </c>
-      <c r="C25" s="60" t="s">
-        <v>1123</v>
-      </c>
-      <c r="G25" s="57" t="s">
-        <v>1176</v>
-      </c>
-      <c r="M25" s="57" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:13" s="93" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="94" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5346,13 +5376,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C63" sqref="C63"/>
+      <selection pane="bottomRight" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5400,7 +5430,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>1038</v>
@@ -5414,7 +5444,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>1016</v>
@@ -5425,7 +5455,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>1039</v>
@@ -5436,7 +5466,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>36</v>
@@ -5447,7 +5477,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>1040</v>
@@ -5458,7 +5488,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C8" s="40" t="s">
         <v>1017</v>
@@ -5469,7 +5499,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>1041</v>
@@ -5484,7 +5514,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C10" s="37" t="s">
         <v>1042</v>
@@ -5499,7 +5529,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C11" s="40" t="s">
         <v>1018</v>
@@ -5510,7 +5540,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C12" s="40" t="s">
         <v>1019</v>
@@ -5521,7 +5551,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>1020</v>
@@ -5532,7 +5562,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C14" s="40" t="s">
         <v>1021</v>
@@ -5698,13 +5728,13 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B33" s="63" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C33" s="62" t="s">
         <v>1107</v>
-      </c>
-      <c r="B33" s="63" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C33" s="62" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5713,290 +5743,280 @@
       <c r="C34" s="62"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="95" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B35" s="96" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C35" s="89" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="95" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B36" s="96" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C36" s="89" t="s">
         <v>1119</v>
       </c>
-      <c r="B35" s="63" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="95" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B37" s="96" t="s">
         <v>1165</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="C37" s="89" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B36" s="63" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="95" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B38" s="96" t="s">
         <v>1166</v>
       </c>
-      <c r="C36" s="57" t="s">
+      <c r="C38" s="89" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="95" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B39" s="96" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C39" s="89" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="95" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B40" s="96" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C40" s="95" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="62" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B37" s="63" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C37" s="57" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="62" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B38" s="90" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C38" s="89" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="62" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B39" s="63" t="s">
-        <v>1168</v>
-      </c>
-      <c r="C39" s="89" t="s">
-        <v>1189</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B40" s="63" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C40" s="89" t="s">
-        <v>1207</v>
-      </c>
-    </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="62" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B41" s="90" t="s">
-        <v>1181</v>
-      </c>
-      <c r="C41" s="89" t="s">
-        <v>1208</v>
-      </c>
+      <c r="B41" s="44"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
-        <v>1119</v>
+        <v>1124</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>1170</v>
+        <v>1125</v>
       </c>
       <c r="C42" s="62" t="s">
-        <v>1123</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="44"/>
+      <c r="A43" s="62" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B43" s="63" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>1128</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="62" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B44" s="63" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C44" s="62" t="s">
-        <v>1128</v>
-      </c>
+      <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="62" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B45" s="63" t="s">
-        <v>1129</v>
-      </c>
-      <c r="C45" s="62" t="s">
+      <c r="A45" s="95" t="s">
         <v>1130</v>
       </c>
+      <c r="B45" s="96" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C45" s="95" t="s">
+        <v>1132</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="44"/>
+      <c r="A46" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B46" s="96" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C46" s="95" t="s">
+        <v>1134</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B47" s="63" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C47" s="62" t="s">
-        <v>1134</v>
+      <c r="A47" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B47" s="96" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C47" s="95" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B48" s="63" t="s">
-        <v>1135</v>
-      </c>
-      <c r="C48" s="62" t="s">
-        <v>1136</v>
+      <c r="A48" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B48" s="96" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C48" s="95" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B49" s="63" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>1138</v>
+      <c r="A49" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B49" s="96" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C49" s="95" t="s">
+        <v>1140</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B50" s="63" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C50" s="62" t="s">
-        <v>1140</v>
+      <c r="A50" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B50" s="96" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C50" s="95" t="s">
+        <v>1142</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B51" s="63" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C51" s="62" t="s">
-        <v>1142</v>
+      <c r="A51" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B51" s="96" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C51" s="95" t="s">
+        <v>1144</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B52" s="63" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C52" s="62" t="s">
-        <v>1144</v>
+      <c r="A52" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B52" s="96" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C52" s="95" t="s">
+        <v>1146</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B53" s="63" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C53" s="62" t="s">
-        <v>1146</v>
+      <c r="A53" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B53" s="96" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C53" s="95" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B54" s="63" t="s">
-        <v>1147</v>
-      </c>
-      <c r="C54" s="62" t="s">
-        <v>1148</v>
+      <c r="A54" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B54" s="96" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C54" s="95" t="s">
+        <v>1150</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B55" s="63" t="s">
-        <v>1149</v>
-      </c>
-      <c r="C55" s="62" t="s">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B56" s="63" t="s">
+      <c r="A55" s="95" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B55" s="96" t="s">
         <v>1151</v>
       </c>
-      <c r="C56" s="62" t="s">
+      <c r="C55" s="95" t="s">
         <v>1152</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="62" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B57" s="63" t="s">
-        <v>1153</v>
-      </c>
-      <c r="C57" s="62" t="s">
-        <v>1154</v>
+      <c r="A57" s="95" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B57" s="96" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C57" s="95" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="95" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B58" s="96" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C58" s="95" t="s">
+        <v>1204</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="93" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B59" s="90" t="s">
-        <v>1198</v>
-      </c>
-      <c r="C59" s="93" t="s">
-        <v>1194</v>
+      <c r="A59" s="95" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B59" s="96" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C59" s="95" t="s">
+        <v>1206</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="93" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B60" s="90" t="s">
-        <v>1200</v>
-      </c>
-      <c r="C60" s="93" t="s">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="93" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B61" s="90" t="s">
-        <v>1199</v>
-      </c>
-      <c r="C61" s="93" t="s">
-        <v>1196</v>
+      <c r="A60" s="95" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B60" s="96" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C60" s="95" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="93" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B62" s="90" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C62" s="93" t="s">
-        <v>1197</v>
-      </c>
+      <c r="B62" s="9"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="9"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F12" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState ref="A907:C935">
-    <sortCondition ref="C907:C935"/>
+  <sortState ref="A905:C933">
+    <sortCondition ref="C905:C933"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -6008,7 +6028,7 @@
   <dimension ref="A1:I4075"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A530" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A536" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J546" sqref="J546"/>
     </sheetView>
   </sheetViews>
@@ -6048,7 +6068,7 @@
         <v>43</v>
       </c>
       <c r="H1" s="86" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -13898,13 +13918,13 @@
     </row>
     <row r="537" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A537" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B537" s="75" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C537" s="74" t="s">
         <v>1067</v>
-      </c>
-      <c r="C537" s="74" t="s">
-        <v>1068</v>
       </c>
       <c r="D537" s="73"/>
       <c r="E537" s="73"/>
@@ -13914,13 +13934,13 @@
     </row>
     <row r="538" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A538" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B538" s="78" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C538" s="77" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="D538" s="73"/>
       <c r="E538" s="73"/>
@@ -13930,13 +13950,13 @@
     </row>
     <row r="539" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A539" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B539" s="75" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C539" s="74" t="s">
         <v>1070</v>
-      </c>
-      <c r="C539" s="74" t="s">
-        <v>1071</v>
       </c>
       <c r="D539" s="73"/>
       <c r="E539" s="73"/>
@@ -13946,13 +13966,13 @@
     </row>
     <row r="540" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A540" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B540" s="75" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C540" s="74" t="s">
         <v>1072</v>
-      </c>
-      <c r="C540" s="74" t="s">
-        <v>1073</v>
       </c>
       <c r="D540" s="73"/>
       <c r="E540" s="73"/>
@@ -13962,13 +13982,13 @@
     </row>
     <row r="541" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A541" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B541" s="75" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C541" s="77" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="D541" s="73"/>
       <c r="E541" s="73"/>
@@ -13978,13 +13998,13 @@
     </row>
     <row r="542" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A542" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B542" s="75" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C542" s="74" t="s">
         <v>1075</v>
-      </c>
-      <c r="C542" s="74" t="s">
-        <v>1076</v>
       </c>
       <c r="D542" s="73"/>
       <c r="E542" s="73"/>
@@ -13994,13 +14014,13 @@
     </row>
     <row r="543" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A543" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B543" s="75" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C543" s="74" t="s">
         <v>1077</v>
-      </c>
-      <c r="C543" s="74" t="s">
-        <v>1078</v>
       </c>
       <c r="D543" s="73"/>
       <c r="E543" s="73"/>
@@ -14010,13 +14030,13 @@
     </row>
     <row r="544" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A544" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B544" s="75" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C544" s="74" t="s">
         <v>1079</v>
-      </c>
-      <c r="C544" s="74" t="s">
-        <v>1080</v>
       </c>
       <c r="D544" s="73"/>
       <c r="E544" s="73"/>
@@ -14026,13 +14046,13 @@
     </row>
     <row r="545" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A545" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B545" s="75" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C545" s="74" t="s">
         <v>1081</v>
-      </c>
-      <c r="C545" s="74" t="s">
-        <v>1082</v>
       </c>
       <c r="D545" s="73"/>
       <c r="E545" s="73"/>
@@ -14042,13 +14062,13 @@
     </row>
     <row r="546" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A546" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B546" s="75" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C546" s="74" t="s">
         <v>1083</v>
-      </c>
-      <c r="C546" s="74" t="s">
-        <v>1084</v>
       </c>
       <c r="D546" s="73"/>
       <c r="E546" s="73"/>
@@ -14058,13 +14078,13 @@
     </row>
     <row r="547" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A547" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B547" s="75" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C547" s="74" t="s">
         <v>1085</v>
-      </c>
-      <c r="C547" s="74" t="s">
-        <v>1086</v>
       </c>
       <c r="D547" s="73"/>
       <c r="E547" s="73"/>
@@ -14074,13 +14094,13 @@
     </row>
     <row r="548" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A548" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B548" s="75" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C548" s="74" t="s">
         <v>1087</v>
-      </c>
-      <c r="C548" s="74" t="s">
-        <v>1088</v>
       </c>
       <c r="D548" s="73"/>
       <c r="E548" s="73"/>
@@ -14090,13 +14110,13 @@
     </row>
     <row r="549" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A549" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B549" s="75" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C549" s="74" t="s">
         <v>1089</v>
-      </c>
-      <c r="C549" s="74" t="s">
-        <v>1090</v>
       </c>
       <c r="D549" s="73"/>
       <c r="E549" s="73"/>
@@ -14106,13 +14126,13 @@
     </row>
     <row r="550" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A550" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B550" s="75" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C550" s="74" t="s">
         <v>1091</v>
-      </c>
-      <c r="C550" s="74" t="s">
-        <v>1092</v>
       </c>
       <c r="D550" s="73"/>
       <c r="E550" s="73"/>
@@ -14122,13 +14142,13 @@
     </row>
     <row r="551" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A551" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B551" s="75" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C551" s="74" t="s">
         <v>1093</v>
-      </c>
-      <c r="C551" s="74" t="s">
-        <v>1094</v>
       </c>
       <c r="D551" s="73"/>
       <c r="E551" s="73"/>
@@ -14138,13 +14158,13 @@
     </row>
     <row r="552" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A552" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B552" s="75" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C552" s="74" t="s">
         <v>1095</v>
-      </c>
-      <c r="C552" s="74" t="s">
-        <v>1096</v>
       </c>
       <c r="D552" s="73"/>
       <c r="E552" s="73"/>
@@ -14154,13 +14174,13 @@
     </row>
     <row r="553" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A553" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B553" s="75" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C553" s="74" t="s">
         <v>1097</v>
-      </c>
-      <c r="C553" s="74" t="s">
-        <v>1098</v>
       </c>
       <c r="D553" s="73"/>
       <c r="E553" s="73"/>
@@ -14170,13 +14190,13 @@
     </row>
     <row r="554" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A554" s="76" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B554" s="75" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C554" s="74" t="s">
         <v>1099</v>
-      </c>
-      <c r="C554" s="74" t="s">
-        <v>1100</v>
       </c>
       <c r="D554" s="73"/>
       <c r="E554" s="73"/>
@@ -30858,8 +30878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30887,16 +30907,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>1102</v>
+        <v>1181</v>
       </c>
       <c r="C2" s="27">
-        <v>201708221</v>
+        <v>201709251</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>1212</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Form M updated with new language on intro note
</commit_message>
<xml_diff>
--- a/M_objeccoes_correcoes/LEGEND_M_objeccoes_correcoes-media/LEGEND_M_objeccoes_correcoes.xlsx
+++ b/M_objeccoes_correcoes/LEGEND_M_objeccoes_correcoes-media/LEGEND_M_objeccoes_correcoes.xlsx
@@ -3581,95 +3581,107 @@
     <t>concat('OC','_',${parcel_id})</t>
   </si>
   <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>Por favor, selecione o resultado para esta parcela</t>
+  </si>
+  <si>
+    <t>party_id</t>
+  </si>
+  <si>
+    <t>Qual é o numero do (co-)titular?</t>
+  </si>
+  <si>
+    <t>party_id_check</t>
+  </si>
+  <si>
+    <t>Por favor, re-digite o número do (co-)titular como confirmação:</t>
+  </si>
+  <si>
+    <t>.=${party_id}</t>
+  </si>
+  <si>
+    <t>O número do titular que reentrou não corresponde à sua primeira entrada. Faça a favor de verificar de novo.</t>
+  </si>
+  <si>
+    <t>${outcome}='change'</t>
+  </si>
+  <si>
+    <t>Novo apelido da pessoa</t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâôàèê]{1,75}$")</t>
+  </si>
+  <si>
+    <t>Resposta invalida - O campo do nome não pode incluir um novo paragrafo. Faça a favor de eliminar qualquer linha adicional.</t>
+  </si>
+  <si>
+    <t>Novo nome da pessoa</t>
+  </si>
+  <si>
+    <t>Mudar o tipo de documento de identificação</t>
+  </si>
+  <si>
+    <t>limites_new_image</t>
+  </si>
+  <si>
+    <t>Tire uma fotografia da parcela no mapa, mostrando claramente a mudança nas limites</t>
+  </si>
+  <si>
+    <t>Mudar o numero de documento</t>
+  </si>
+  <si>
+    <t>certify</t>
+  </si>
+  <si>
+    <t>Todos os detalhes estão corretos e confirmados</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>Foi feita uma alteração aos detalhes do(s) (co-)titular(es) ou as limites da parcela</t>
+  </si>
+  <si>
+    <t>disputed</t>
+  </si>
+  <si>
+    <t>Foi feita uma objecção que necessita uma resolução ainda</t>
+  </si>
+  <si>
+    <t>unconfirmed</t>
+  </si>
+  <si>
+    <t>O titular não confirmou os seus detalhes durante o período de O &amp; C</t>
+  </si>
+  <si>
     <t>&lt;br/&gt; &lt;span style="color:#57b055"&gt;${my_form_name}&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;Este formulário é utilizado para gravar os resultados de processo de Objecções e Correções.
 O técnico pode usar o formulário &lt;br/&gt; &lt;span style="color:#57b055"&gt;depois de conclusão da publicação do edital&lt;/span&gt;.
-O formulário é usado para reportar a necessidade de mudar ou a configuração das parcelas ou mudanças na informação relacionada sobre os titulares. 
-&lt;span style="color:#FF0000"&gt;Se os detalhes de mais de um titular dos co-titulares precisam de ser alterados, o formulário deve ser preenchido uma vez para cada titular&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;
+O formulário é usado para reportar:
+- a necessidade de mudar a configuração dos limites de parcelas
+ou
+- mudanças na informação publicada no edital, relacionada aos titulares
+ou
+- para confirmar a informação publicada no edital, relacionada aos titulares
+&lt;span style="color:#FF0000"&gt;Se houver mais de um titular para uma parcela, o formulário deve ser preenchido uma vez para cada titular&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;
 Por favor deslizar para a frente para continuar.</t>
-  </si>
-  <si>
-    <t>outcome</t>
-  </si>
-  <si>
-    <t>Por favor, selecione o resultado para esta parcela</t>
-  </si>
-  <si>
-    <t>party_id</t>
-  </si>
-  <si>
-    <t>Qual é o numero do (co-)titular?</t>
-  </si>
-  <si>
-    <t>party_id_check</t>
-  </si>
-  <si>
-    <t>Por favor, re-digite o número do (co-)titular como confirmação:</t>
-  </si>
-  <si>
-    <t>.=${party_id}</t>
-  </si>
-  <si>
-    <t>O número do titular que reentrou não corresponde à sua primeira entrada. Faça a favor de verificar de novo.</t>
-  </si>
-  <si>
-    <t>${outcome}='change'</t>
-  </si>
-  <si>
-    <t>Novo apelido da pessoa</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâôàèê]{1,75}$")</t>
-  </si>
-  <si>
-    <t>Resposta invalida - O campo do nome não pode incluir um novo paragrafo. Faça a favor de eliminar qualquer linha adicional.</t>
-  </si>
-  <si>
-    <t>Novo nome da pessoa</t>
-  </si>
-  <si>
-    <t>Mudar o tipo de documento de identificação</t>
-  </si>
-  <si>
-    <t>limites_new_image</t>
-  </si>
-  <si>
-    <t>Tire uma fotografia da parcela no mapa, mostrando claramente a mudança nas limites</t>
-  </si>
-  <si>
-    <t>Mudar o numero de documento</t>
-  </si>
-  <si>
-    <t>certify</t>
-  </si>
-  <si>
-    <t>Todos os detalhes estão corretos e confirmados</t>
-  </si>
-  <si>
-    <t>change</t>
-  </si>
-  <si>
-    <t>Foi feita uma alteração aos detalhes do(s) (co-)titular(es) ou as limites da parcela</t>
-  </si>
-  <si>
-    <t>disputed</t>
-  </si>
-  <si>
-    <t>Foi feita uma objecção que necessita uma resolução ainda</t>
-  </si>
-  <si>
-    <t>unconfirmed</t>
-  </si>
-  <si>
-    <t>O titular não confirmou os seus detalhes durante o período de O &amp; C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3844,405 +3856,405 @@
   </borders>
   <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -4251,37 +4263,37 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="238" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="238" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="238" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="239">
@@ -4863,10 +4875,10 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4955,15 +4967,15 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="40" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="40" customFormat="1" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>1045</v>
       </c>
       <c r="B5" s="48" t="s">
         <v>1046</v>
       </c>
-      <c r="C5" s="90" t="s">
-        <v>1183</v>
+      <c r="C5" s="96" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4997,10 +5009,10 @@
         <v>1049</v>
       </c>
       <c r="H7" s="89" t="s">
+        <v>1193</v>
+      </c>
+      <c r="I7" s="89" t="s">
         <v>1194</v>
-      </c>
-      <c r="I7" s="89" t="s">
-        <v>1195</v>
       </c>
       <c r="J7" s="40" t="s">
         <v>21</v>
@@ -5147,11 +5159,11 @@
       <c r="A15" s="89" t="s">
         <v>1179</v>
       </c>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="90" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C15" s="91" t="s">
         <v>1184</v>
-      </c>
-      <c r="C15" s="92" t="s">
-        <v>1185</v>
       </c>
       <c r="J15" s="89" t="s">
         <v>21</v>
@@ -5161,16 +5173,16 @@
       <c r="A16" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="90" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C16" s="89" t="s">
         <v>1186</v>
-      </c>
-      <c r="C16" s="89" t="s">
-        <v>1187</v>
       </c>
       <c r="J16" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="93" t="s">
+      <c r="L16" s="92" t="s">
         <v>1110</v>
       </c>
     </row>
@@ -5178,22 +5190,22 @@
       <c r="A17" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="90" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C17" s="91" t="s">
         <v>1188</v>
       </c>
-      <c r="C17" s="92" t="s">
+      <c r="H17" s="89" t="s">
         <v>1189</v>
       </c>
-      <c r="H17" s="89" t="s">
+      <c r="I17" s="89" t="s">
         <v>1190</v>
-      </c>
-      <c r="I17" s="89" t="s">
-        <v>1191</v>
       </c>
       <c r="J17" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="93" t="s">
+      <c r="L17" s="92" t="s">
         <v>1110</v>
       </c>
     </row>
@@ -5201,14 +5213,14 @@
       <c r="A18" s="89" t="s">
         <v>1116</v>
       </c>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="90" t="s">
         <v>1117</v>
       </c>
-      <c r="C18" s="92" t="s">
+      <c r="C18" s="91" t="s">
         <v>1122</v>
       </c>
-      <c r="G18" s="93" t="s">
-        <v>1192</v>
+      <c r="G18" s="92" t="s">
+        <v>1191</v>
       </c>
       <c r="J18" s="89" t="s">
         <v>21</v>
@@ -5218,20 +5230,20 @@
       <c r="A19" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="90" t="s">
         <v>1157</v>
       </c>
-      <c r="C19" s="92" t="s">
-        <v>1193</v>
+      <c r="C19" s="91" t="s">
+        <v>1192</v>
       </c>
       <c r="G19" s="89" t="s">
         <v>1169</v>
       </c>
       <c r="H19" s="89" t="s">
+        <v>1193</v>
+      </c>
+      <c r="I19" s="89" t="s">
         <v>1194</v>
-      </c>
-      <c r="I19" s="89" t="s">
-        <v>1195</v>
       </c>
       <c r="J19" s="89" t="s">
         <v>21</v>
@@ -5241,20 +5253,20 @@
       <c r="A20" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="91" t="s">
+      <c r="B20" s="90" t="s">
         <v>1158</v>
       </c>
-      <c r="C20" s="92" t="s">
-        <v>1196</v>
+      <c r="C20" s="91" t="s">
+        <v>1195</v>
       </c>
       <c r="G20" s="89" t="s">
         <v>1170</v>
       </c>
       <c r="H20" s="89" t="s">
+        <v>1193</v>
+      </c>
+      <c r="I20" s="89" t="s">
         <v>1194</v>
-      </c>
-      <c r="I20" s="89" t="s">
-        <v>1195</v>
       </c>
       <c r="J20" s="89" t="s">
         <v>21</v>
@@ -5264,10 +5276,10 @@
       <c r="A21" s="89" t="s">
         <v>1129</v>
       </c>
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="90" t="s">
         <v>1159</v>
       </c>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="91" t="s">
         <v>1123</v>
       </c>
       <c r="G21" s="89" t="s">
@@ -5276,7 +5288,7 @@
       <c r="J21" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="93" t="s">
+      <c r="L21" s="92" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5284,11 +5296,11 @@
       <c r="A22" s="89" t="s">
         <v>1153</v>
       </c>
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="90" t="s">
         <v>1160</v>
       </c>
-      <c r="C22" s="92" t="s">
-        <v>1197</v>
+      <c r="C22" s="91" t="s">
+        <v>1196</v>
       </c>
       <c r="G22" s="89" t="s">
         <v>1172</v>
@@ -5296,7 +5308,7 @@
       <c r="J22" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="93" t="s">
+      <c r="L22" s="92" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5304,7 +5316,7 @@
       <c r="A23" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="91" t="s">
+      <c r="B23" s="90" t="s">
         <v>1161</v>
       </c>
       <c r="C23" s="89" t="s">
@@ -5327,10 +5339,10 @@
       <c r="A24" s="89" t="s">
         <v>1043</v>
       </c>
-      <c r="B24" s="91" t="s">
+      <c r="B24" s="90" t="s">
         <v>1162</v>
       </c>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="91" t="s">
         <v>1121</v>
       </c>
       <c r="G24" s="89" t="s">
@@ -5347,11 +5359,11 @@
       <c r="A25" s="89" t="s">
         <v>1180</v>
       </c>
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="90" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C25" s="91" t="s">
         <v>1198</v>
-      </c>
-      <c r="C25" s="92" t="s">
-        <v>1199</v>
       </c>
       <c r="G25" s="89" t="s">
         <v>1174</v>
@@ -5360,11 +5372,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="93" t="s">
+    <row r="26" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="93" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5382,7 +5394,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5743,10 +5755,10 @@
       <c r="C34" s="62"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="95" t="s">
+      <c r="A35" s="94" t="s">
         <v>1117</v>
       </c>
-      <c r="B35" s="96" t="s">
+      <c r="B35" s="95" t="s">
         <v>1163</v>
       </c>
       <c r="C35" s="89" t="s">
@@ -5754,10 +5766,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="95" t="s">
+      <c r="A36" s="94" t="s">
         <v>1117</v>
       </c>
-      <c r="B36" s="96" t="s">
+      <c r="B36" s="95" t="s">
         <v>1164</v>
       </c>
       <c r="C36" s="89" t="s">
@@ -5765,10 +5777,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="95" t="s">
+      <c r="A37" s="94" t="s">
         <v>1117</v>
       </c>
-      <c r="B37" s="96" t="s">
+      <c r="B37" s="95" t="s">
         <v>1165</v>
       </c>
       <c r="C37" s="89" t="s">
@@ -5776,35 +5788,35 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="95" t="s">
+      <c r="A38" s="94" t="s">
         <v>1117</v>
       </c>
-      <c r="B38" s="96" t="s">
+      <c r="B38" s="95" t="s">
         <v>1166</v>
       </c>
       <c r="C38" s="89" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="95" t="s">
+      <c r="A39" s="94" t="s">
         <v>1117</v>
       </c>
-      <c r="B39" s="96" t="s">
+      <c r="B39" s="95" t="s">
         <v>1167</v>
       </c>
       <c r="C39" s="89" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="95" t="s">
+      <c r="A40" s="94" t="s">
         <v>1117</v>
       </c>
-      <c r="B40" s="96" t="s">
+      <c r="B40" s="95" t="s">
         <v>1168</v>
       </c>
-      <c r="C40" s="95" t="s">
+      <c r="C40" s="94" t="s">
         <v>1121</v>
       </c>
     </row>
@@ -5837,168 +5849,168 @@
       <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="95" t="s">
+      <c r="A45" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B45" s="96" t="s">
+      <c r="B45" s="95" t="s">
         <v>1131</v>
       </c>
-      <c r="C45" s="95" t="s">
+      <c r="C45" s="94" t="s">
         <v>1132</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="95" t="s">
+      <c r="A46" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B46" s="96" t="s">
+      <c r="B46" s="95" t="s">
         <v>1133</v>
       </c>
-      <c r="C46" s="95" t="s">
+      <c r="C46" s="94" t="s">
         <v>1134</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="95" t="s">
+      <c r="A47" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B47" s="96" t="s">
+      <c r="B47" s="95" t="s">
         <v>1135</v>
       </c>
-      <c r="C47" s="95" t="s">
+      <c r="C47" s="94" t="s">
         <v>1136</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="95" t="s">
+      <c r="A48" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B48" s="96" t="s">
+      <c r="B48" s="95" t="s">
         <v>1137</v>
       </c>
-      <c r="C48" s="95" t="s">
+      <c r="C48" s="94" t="s">
         <v>1138</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="95" t="s">
+      <c r="A49" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B49" s="96" t="s">
+      <c r="B49" s="95" t="s">
         <v>1139</v>
       </c>
-      <c r="C49" s="95" t="s">
+      <c r="C49" s="94" t="s">
         <v>1140</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="95" t="s">
+      <c r="A50" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B50" s="96" t="s">
+      <c r="B50" s="95" t="s">
         <v>1141</v>
       </c>
-      <c r="C50" s="95" t="s">
+      <c r="C50" s="94" t="s">
         <v>1142</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="95" t="s">
+      <c r="A51" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B51" s="96" t="s">
+      <c r="B51" s="95" t="s">
         <v>1143</v>
       </c>
-      <c r="C51" s="95" t="s">
+      <c r="C51" s="94" t="s">
         <v>1144</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="95" t="s">
+      <c r="A52" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B52" s="96" t="s">
+      <c r="B52" s="95" t="s">
         <v>1145</v>
       </c>
-      <c r="C52" s="95" t="s">
+      <c r="C52" s="94" t="s">
         <v>1146</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="95" t="s">
+      <c r="A53" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B53" s="96" t="s">
+      <c r="B53" s="95" t="s">
         <v>1147</v>
       </c>
-      <c r="C53" s="95" t="s">
+      <c r="C53" s="94" t="s">
         <v>1148</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="95" t="s">
+      <c r="A54" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B54" s="96" t="s">
+      <c r="B54" s="95" t="s">
         <v>1149</v>
       </c>
-      <c r="C54" s="95" t="s">
+      <c r="C54" s="94" t="s">
         <v>1150</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="95" t="s">
+      <c r="A55" s="94" t="s">
         <v>1130</v>
       </c>
-      <c r="B55" s="96" t="s">
+      <c r="B55" s="95" t="s">
         <v>1151</v>
       </c>
-      <c r="C55" s="95" t="s">
+      <c r="C55" s="94" t="s">
         <v>1152</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="95" t="s">
+      <c r="A57" s="94" t="s">
         <v>1178</v>
       </c>
-      <c r="B57" s="96" t="s">
+      <c r="B57" s="95" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C57" s="94" t="s">
         <v>1201</v>
       </c>
-      <c r="C57" s="95" t="s">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="94" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B58" s="95" t="s">
         <v>1202</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="95" t="s">
+      <c r="C58" s="94" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="94" t="s">
         <v>1178</v>
       </c>
-      <c r="B58" s="96" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C58" s="95" t="s">
+      <c r="B59" s="95" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="95" t="s">
+      <c r="C59" s="94" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="94" t="s">
         <v>1178</v>
       </c>
-      <c r="B59" s="96" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C59" s="95" t="s">
+      <c r="B60" s="95" t="s">
         <v>1206</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="95" t="s">
-        <v>1178</v>
-      </c>
-      <c r="B60" s="96" t="s">
+      <c r="C60" s="94" t="s">
         <v>1207</v>
-      </c>
-      <c r="C60" s="95" t="s">
-        <v>1208</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -30879,7 +30891,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30913,7 +30925,7 @@
         <v>1181</v>
       </c>
       <c r="C2" s="27">
-        <v>201709251</v>
+        <v>201709261</v>
       </c>
       <c r="D2" s="89" t="s">
         <v>1182</v>

</xml_diff>